<commit_message>
updating model.  latests news is 50-1 stock split
</commit_message>
<xml_diff>
--- a/CMG.xlsx
+++ b/CMG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Library/CloudStorage/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06625BCA-70CA-5742-8D0A-6ED073AF6996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCB82D0-101D-344F-9C39-BD66ACA8A7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14960" yWindow="500" windowWidth="36240" windowHeight="28300" xr2:uid="{CA65A239-F34F-E142-B5DA-63A84FA73A6D}"/>
   </bookViews>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="208">
   <si>
     <t>Q119</t>
   </si>
@@ -870,7 +870,16 @@
     <t>Meati Foods</t>
   </si>
   <si>
-    <t>Cultivate Next Fund</t>
+    <t xml:space="preserve">50-1 stock split </t>
+  </si>
+  <si>
+    <t>Cultivate Next Fund -- 1st in co history</t>
+  </si>
+  <si>
+    <t>Al pastor  --- shit is nasty imo</t>
+  </si>
+  <si>
+    <t>Years alive</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1012,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1"/>
@@ -1177,6 +1186,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1638,17 +1649,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3C8013-9F59-6546-8AA7-191A6CA15E5B}">
-  <dimension ref="A1:O105"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="234" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8" style="3" customWidth="1"/>
     <col min="4" max="4" width="9" style="3" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -1700,12 +1711,19 @@
         <v>12</v>
       </c>
       <c r="G4" s="4">
-        <v>2598</v>
+        <v>2904.98</v>
       </c>
       <c r="J4" s="4"/>
       <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13">
+      <c r="B5" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="76">
+        <f ca="1">(TODAY()-C3)/365</f>
+        <v>30.712328767123289</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1724,7 +1742,7 @@
       </c>
       <c r="G6" s="4">
         <f>+G4*G5</f>
-        <v>71240197062</v>
+        <v>79657947521.619995</v>
       </c>
       <c r="J6" s="4"/>
       <c r="M6" s="9"/>
@@ -1763,7 +1781,7 @@
       </c>
       <c r="G9" s="4">
         <f>+G6-G7+G8</f>
-        <v>70679588062</v>
+        <v>79097338521.619995</v>
       </c>
       <c r="J9" s="4"/>
       <c r="M9" s="10"/>
@@ -1792,331 +1810,341 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="57">
-        <v>45350</v>
-      </c>
-      <c r="C15" t="s">
+        <v>45370</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="57">
-        <v>45293</v>
+        <v>45363</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="57">
+        <v>45350</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="57">
+        <v>45293</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="57">
         <v>45273</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="67">
-        <v>44845</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="67">
-        <v>44831</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="67">
-        <v>44817</v>
+        <v>44845</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="67">
-        <v>44811</v>
+        <v>44831</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="67">
-        <v>44803</v>
+        <v>44817</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="67">
-        <v>44795</v>
+        <v>44811</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="67">
-        <v>44763</v>
+        <v>44803</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="67">
-        <v>44740</v>
+        <v>44795</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="67">
-        <v>44728</v>
+        <v>44763</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="2:3">
       <c r="B27" s="67">
-        <v>44721</v>
+        <v>44740</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="67">
-        <v>44683</v>
+        <v>44728</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" s="67">
+        <v>44721</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="67">
+        <v>44683</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="67">
         <v>44677</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="68">
-        <v>44670</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="68">
-        <v>44656</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" s="68">
-        <v>44651</v>
+        <v>44670</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="68">
-        <v>44648</v>
+        <v>44656</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="68">
-        <v>44636</v>
+        <v>44651</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="68">
-        <v>44630</v>
+        <v>44648</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="68">
-        <v>44615</v>
+        <v>44636</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="2:3">
       <c r="B37" s="68">
-        <v>44607</v>
+        <v>44630</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="2:3">
       <c r="B38" s="68">
-        <v>44564</v>
+        <v>44615</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="2:3">
       <c r="B39" s="68">
-        <v>44546</v>
+        <v>44607</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="2:3">
       <c r="B40" s="68">
-        <v>44448</v>
+        <v>44564</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="2:3">
       <c r="B41" s="68">
-        <v>44440</v>
+        <v>44546</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="2:3">
       <c r="B42" s="68">
-        <v>44427</v>
+        <v>44448</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="2:3">
       <c r="B43" s="68">
-        <v>44377</v>
+        <v>44440</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="68">
+        <v>44427</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="68">
+        <v>44377</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" s="68">
         <v>44326</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="67">
+    <row r="47" spans="2:3">
+      <c r="B47" s="67">
         <v>44280</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="68"/>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="68"/>
     </row>
     <row r="48" spans="2:3">
       <c r="B48" s="68"/>
     </row>
-    <row r="51" spans="2:15">
-      <c r="B51" s="7" t="s">
+    <row r="49" spans="2:15">
+      <c r="B49" s="68"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="68"/>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
-      <c r="B52" s="7" t="s">
+    <row r="54" spans="2:15">
+      <c r="B54" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
-      <c r="B53" s="2" t="s">
+    <row r="55" spans="2:15">
+      <c r="B55" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
-      <c r="B54" s="3" t="s">
+    <row r="56" spans="2:15">
+      <c r="B56" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
-      <c r="L55" s="7"/>
-      <c r="N55" s="7"/>
-    </row>
-    <row r="56" spans="2:15">
-      <c r="B56" s="7" t="s">
+    <row r="57" spans="2:15">
+      <c r="L57" s="7"/>
+      <c r="N57" s="7"/>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="N56" s="12"/>
-    </row>
-    <row r="57" spans="2:15">
-      <c r="B57" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="N57" s="12"/>
-    </row>
-    <row r="58" spans="2:15">
-      <c r="B58" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="N58" s="12"/>
     </row>
     <row r="59" spans="2:15">
       <c r="B59" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="10"/>
+        <v>189</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="N59" s="12"/>
     </row>
     <row r="60" spans="2:15">
       <c r="B60" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="N60" s="12"/>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="B61" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="13"/>
+      <c r="O61" s="10"/>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="N60" s="12"/>
-    </row>
-    <row r="61" spans="2:15">
-      <c r="N61" s="12"/>
-    </row>
-    <row r="62" spans="2:15">
       <c r="N62" s="12"/>
     </row>
     <row r="63" spans="2:15">
@@ -2242,39 +2270,47 @@
     <row r="103" spans="13:14">
       <c r="N103" s="12"/>
     </row>
+    <row r="104" spans="13:14">
+      <c r="N104" s="12"/>
+    </row>
     <row r="105" spans="13:14">
-      <c r="M105" s="4"/>
+      <c r="N105" s="12"/>
+    </row>
+    <row r="107" spans="13:14">
+      <c r="M107" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B40" r:id="rId1" display="9/9/21 Press Release" xr:uid="{D879A47D-CEDE-6B45-9E60-9F54FB18B685}"/>
-    <hyperlink ref="B41" r:id="rId2" display="9/1/21 Press Release" xr:uid="{919BA319-D27F-5F45-A159-BD7F47F2F59D}"/>
-    <hyperlink ref="B42" r:id="rId3" display="8/19/21 Press Release " xr:uid="{B211C8DC-3A52-F14F-8F6D-24C0F5F95485}"/>
-    <hyperlink ref="B43" r:id="rId4" display="6/30/21 Press Release" xr:uid="{33BCD7E2-316F-0A41-B77C-80F8C21D0669}"/>
-    <hyperlink ref="B44" r:id="rId5" display="5/10/21 Press Release" xr:uid="{39EC7DB8-A0BC-B149-906C-A4D8AE9C2474}"/>
-    <hyperlink ref="B38" r:id="rId6" display="1/3/2022 Press release" xr:uid="{27C89C1F-6A3B-8E47-9D36-8C4F95C3DD23}"/>
-    <hyperlink ref="B39" r:id="rId7" display="12/16/21 Press release" xr:uid="{332C27BD-6179-A44B-82BA-1BB3D044EC05}"/>
-    <hyperlink ref="B34" r:id="rId8" display="3/16/2022 Press Release" xr:uid="{3D9CDEB0-1E08-1E46-BAE4-80C186F12D19}"/>
-    <hyperlink ref="B53" r:id="rId9" xr:uid="{9BE232BB-5FDC-6C4F-A32E-5212308C52F0}"/>
-    <hyperlink ref="B35" r:id="rId10" display="3/10/22 Press Release" xr:uid="{993F6CD6-AF6A-D34E-A97A-0883743F6E97}"/>
-    <hyperlink ref="B37" r:id="rId11" display="2/15/2022 Press Release" xr:uid="{40FC8D02-2B58-E347-B032-7BA7EFAAD1CA}"/>
+    <hyperlink ref="B42" r:id="rId1" display="9/9/21 Press Release" xr:uid="{D879A47D-CEDE-6B45-9E60-9F54FB18B685}"/>
+    <hyperlink ref="B43" r:id="rId2" display="9/1/21 Press Release" xr:uid="{919BA319-D27F-5F45-A159-BD7F47F2F59D}"/>
+    <hyperlink ref="B44" r:id="rId3" display="8/19/21 Press Release " xr:uid="{B211C8DC-3A52-F14F-8F6D-24C0F5F95485}"/>
+    <hyperlink ref="B45" r:id="rId4" display="6/30/21 Press Release" xr:uid="{33BCD7E2-316F-0A41-B77C-80F8C21D0669}"/>
+    <hyperlink ref="B46" r:id="rId5" display="5/10/21 Press Release" xr:uid="{39EC7DB8-A0BC-B149-906C-A4D8AE9C2474}"/>
+    <hyperlink ref="B40" r:id="rId6" display="1/3/2022 Press release" xr:uid="{27C89C1F-6A3B-8E47-9D36-8C4F95C3DD23}"/>
+    <hyperlink ref="B41" r:id="rId7" display="12/16/21 Press release" xr:uid="{332C27BD-6179-A44B-82BA-1BB3D044EC05}"/>
+    <hyperlink ref="B36" r:id="rId8" display="3/16/2022 Press Release" xr:uid="{3D9CDEB0-1E08-1E46-BAE4-80C186F12D19}"/>
+    <hyperlink ref="B55" r:id="rId9" xr:uid="{9BE232BB-5FDC-6C4F-A32E-5212308C52F0}"/>
+    <hyperlink ref="B37" r:id="rId10" display="3/10/22 Press Release" xr:uid="{993F6CD6-AF6A-D34E-A97A-0883743F6E97}"/>
+    <hyperlink ref="B39" r:id="rId11" display="2/15/2022 Press Release" xr:uid="{40FC8D02-2B58-E347-B032-7BA7EFAAD1CA}"/>
     <hyperlink ref="A1" location="Model!A1" display="Model" xr:uid="{4EBDF202-A121-B14F-A255-3F8E62B44989}"/>
-    <hyperlink ref="B30" r:id="rId12" display="4/19/22 Press Release" xr:uid="{4A0C956C-3152-864B-91A8-4119706762C5}"/>
-    <hyperlink ref="B33" r:id="rId13" display="3/28/22 Press Release" xr:uid="{E98A3860-CE2C-D346-A7F8-3BFECB77F349}"/>
-    <hyperlink ref="B31" r:id="rId14" display="4/5/22 Press Release" xr:uid="{0BE5ACE2-4857-3B4D-A854-8D959D99B602}"/>
-    <hyperlink ref="B29" r:id="rId15" display="4/26/22 Press Release" xr:uid="{F45703FF-7DA6-AD43-A4AB-DA9E06AC4711}"/>
-    <hyperlink ref="B28" r:id="rId16" display="5/2/22 Press Release" xr:uid="{064F4BA5-C4A3-394A-A224-77908E3229CD}"/>
-    <hyperlink ref="B27" r:id="rId17" display="6/9/22 Press Release" xr:uid="{98142C7F-2AA7-8B44-B252-2DE623CB2A48}"/>
-    <hyperlink ref="B26" r:id="rId18" display="6/16/22 Press Release" xr:uid="{C0CF27D7-F5D7-D44D-A046-6D01F37E2A6A}"/>
-    <hyperlink ref="B25" r:id="rId19" display="6/28/22 Press Release" xr:uid="{236EE2B4-06FC-FC43-BCD9-B55CD85EF132}"/>
-    <hyperlink ref="B18" r:id="rId20" display="10/11/2022 Press Releases" xr:uid="{58D60953-E809-8344-80E4-753831B5BCCD}"/>
-    <hyperlink ref="B19" r:id="rId21" display="9/27/2022 Press Release" xr:uid="{06E23F18-D0BF-1441-8ECB-A0DF37C02A7E}"/>
-    <hyperlink ref="B20" r:id="rId22" display="9/13/22 Press Release" xr:uid="{31796C53-3353-614C-850C-37223269C65A}"/>
-    <hyperlink ref="B21" r:id="rId23" display="9/7/22 Press Release" xr:uid="{F5A9EBA8-65D3-B145-BFD3-96A9517114BB}"/>
-    <hyperlink ref="B16" r:id="rId24" display="https://ir.chipotle.com/2024-01-02-CHIPOTLE-AND-STRAVA-TEAM-UP-TO-HELP-FANS-ACHIEVE-WELLNESS-GOALS-ALL-JANUARY" xr:uid="{8F61C397-6067-AC4B-B494-83E922F1BE68}"/>
-    <hyperlink ref="B17" r:id="rId25" display="https://ir.chipotle.com/2023-12-13-CHIPOTLE-INVESTS-IN-AUTONOMOUS-AGRICULTURAL-ROBOTS-AND-CLIMATE-SMART-FERTILIZER-TO-IMPROVE-THE-FUTURE-OF-FARMING" xr:uid="{F5AC78B6-94FC-8546-AB05-921EDE6AB4EE}"/>
-    <hyperlink ref="B45" r:id="rId26" display="https://ir.chipotle.com/2021-03-25-Chipotle-Invests-In-Leading-Autonomous-Delivery-Company-Nuro" xr:uid="{42BFF284-5C82-4F42-B97C-204926615DF4}"/>
-    <hyperlink ref="B15" r:id="rId27" display="https://ir.chipotle.com/2024-02-28-CHIPOTLE-DOUBLES-ITS-COMMITMENT-TO-THE-CULTIVATE-NEXT-VENTURE-FUND-TO-100-MILLION,-MARKING-ITS-TWO-YEAR-ANNIVERSARY" xr:uid="{6B02CC92-51C3-B645-B764-8CD662CC60BB}"/>
+    <hyperlink ref="B32" r:id="rId12" display="4/19/22 Press Release" xr:uid="{4A0C956C-3152-864B-91A8-4119706762C5}"/>
+    <hyperlink ref="B35" r:id="rId13" display="3/28/22 Press Release" xr:uid="{E98A3860-CE2C-D346-A7F8-3BFECB77F349}"/>
+    <hyperlink ref="B33" r:id="rId14" display="4/5/22 Press Release" xr:uid="{0BE5ACE2-4857-3B4D-A854-8D959D99B602}"/>
+    <hyperlink ref="B31" r:id="rId15" display="4/26/22 Press Release" xr:uid="{F45703FF-7DA6-AD43-A4AB-DA9E06AC4711}"/>
+    <hyperlink ref="B30" r:id="rId16" display="5/2/22 Press Release" xr:uid="{064F4BA5-C4A3-394A-A224-77908E3229CD}"/>
+    <hyperlink ref="B29" r:id="rId17" display="6/9/22 Press Release" xr:uid="{98142C7F-2AA7-8B44-B252-2DE623CB2A48}"/>
+    <hyperlink ref="B28" r:id="rId18" display="6/16/22 Press Release" xr:uid="{C0CF27D7-F5D7-D44D-A046-6D01F37E2A6A}"/>
+    <hyperlink ref="B27" r:id="rId19" display="6/28/22 Press Release" xr:uid="{236EE2B4-06FC-FC43-BCD9-B55CD85EF132}"/>
+    <hyperlink ref="B20" r:id="rId20" display="10/11/2022 Press Releases" xr:uid="{58D60953-E809-8344-80E4-753831B5BCCD}"/>
+    <hyperlink ref="B21" r:id="rId21" display="9/27/2022 Press Release" xr:uid="{06E23F18-D0BF-1441-8ECB-A0DF37C02A7E}"/>
+    <hyperlink ref="B22" r:id="rId22" display="9/13/22 Press Release" xr:uid="{31796C53-3353-614C-850C-37223269C65A}"/>
+    <hyperlink ref="B23" r:id="rId23" display="9/7/22 Press Release" xr:uid="{F5A9EBA8-65D3-B145-BFD3-96A9517114BB}"/>
+    <hyperlink ref="B18" r:id="rId24" display="https://ir.chipotle.com/2024-01-02-CHIPOTLE-AND-STRAVA-TEAM-UP-TO-HELP-FANS-ACHIEVE-WELLNESS-GOALS-ALL-JANUARY" xr:uid="{8F61C397-6067-AC4B-B494-83E922F1BE68}"/>
+    <hyperlink ref="B19" r:id="rId25" display="https://ir.chipotle.com/2023-12-13-CHIPOTLE-INVESTS-IN-AUTONOMOUS-AGRICULTURAL-ROBOTS-AND-CLIMATE-SMART-FERTILIZER-TO-IMPROVE-THE-FUTURE-OF-FARMING" xr:uid="{F5AC78B6-94FC-8546-AB05-921EDE6AB4EE}"/>
+    <hyperlink ref="B47" r:id="rId26" display="https://ir.chipotle.com/2021-03-25-Chipotle-Invests-In-Leading-Autonomous-Delivery-Company-Nuro" xr:uid="{42BFF284-5C82-4F42-B97C-204926615DF4}"/>
+    <hyperlink ref="B17" r:id="rId27" display="https://ir.chipotle.com/2024-02-28-CHIPOTLE-DOUBLES-ITS-COMMITMENT-TO-THE-CULTIVATE-NEXT-VENTURE-FUND-TO-100-MILLION,-MARKING-ITS-TWO-YEAR-ANNIVERSARY" xr:uid="{6B02CC92-51C3-B645-B764-8CD662CC60BB}"/>
+    <hyperlink ref="B15" r:id="rId28" display="https://ir.chipotle.com/2024-03-19-CHIPOTLE-BOARD-OF-DIRECTORS-APPROVES-50-FOR-1-STOCK-SPLIT" xr:uid="{B08C3402-BE9C-A34F-ACB4-1730ED1C4966}"/>
+    <hyperlink ref="B16" r:id="rId29" display="https://ir.chipotle.com/2024-03-12-CHICKEN-AL-PASTOR-IS-BACK-CHIPOTLE-REINTRODUCES-ONE-OF-ITS-MOST-POPULAR-MENU-INNOVATIONS" xr:uid="{14879690-4BED-4546-BC50-DB312E87F222}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2284,11 +2320,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31B3FB4-BD2A-5E41-95A2-2CC4EACD5DFD}">
   <dimension ref="B1:IV174"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="AZ4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BG7" sqref="BG7"/>
+      <selection pane="bottomRight" activeCell="BU34" sqref="BU34:BU42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2305,7 +2341,8 @@
     <col min="28" max="28" width="10" style="17" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="38" width="3.6640625" style="17" customWidth="1"/>
+    <col min="31" max="31" width="6.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="38" width="3.6640625" style="17" customWidth="1"/>
     <col min="39" max="40" width="7.6640625" style="20" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="41" max="50" width="9.1640625" style="20" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="51" max="52" width="9.1640625" style="20" bestFit="1" customWidth="1"/>
@@ -2428,7 +2465,9 @@
       <c r="AB2" s="17"/>
       <c r="AC2" s="17"/>
       <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
+      <c r="AE2" s="17">
+        <v>45406</v>
+      </c>
       <c r="AF2" s="17"/>
       <c r="AG2" s="17"/>
       <c r="AH2" s="17"/>
@@ -7443,7 +7482,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="2:73">
+    <row r="33" spans="2:71">
       <c r="B33" s="4" t="s">
         <v>19</v>
       </c>
@@ -7515,7 +7554,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="34" spans="2:73" s="21" customFormat="1">
+    <row r="34" spans="2:71" s="21" customFormat="1">
       <c r="B34" s="10" t="s">
         <v>20</v>
       </c>
@@ -7714,7 +7753,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:73">
+    <row r="35" spans="2:71">
       <c r="B35" s="4" t="s">
         <v>21</v>
       </c>
@@ -7823,7 +7862,7 @@
         <v>69515289.672806218</v>
       </c>
     </row>
-    <row r="36" spans="2:73">
+    <row r="36" spans="2:71">
       <c r="B36" s="4" t="s">
         <v>22</v>
       </c>
@@ -7932,7 +7971,7 @@
         <v>560609</v>
       </c>
     </row>
-    <row r="37" spans="2:73">
+    <row r="37" spans="2:71">
       <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
@@ -8044,12 +8083,8 @@
         <f>+BS35+BS36</f>
         <v>70075898.672806218</v>
       </c>
-      <c r="BU37" s="20">
-        <f>+BS37/BG27</f>
-        <v>25.88188430281815</v>
-      </c>
-    </row>
-    <row r="38" spans="2:73">
+    </row>
+    <row r="38" spans="2:71">
       <c r="B38" s="4" t="s">
         <v>24</v>
       </c>
@@ -8160,7 +8195,7 @@
         <v>27421.169000000002</v>
       </c>
     </row>
-    <row r="39" spans="2:73">
+    <row r="39" spans="2:71">
       <c r="B39" s="4" t="s">
         <v>25</v>
       </c>
@@ -8269,17 +8304,17 @@
         <v>2555.5401621574269</v>
       </c>
     </row>
-    <row r="40" spans="2:73">
+    <row r="40" spans="2:71">
       <c r="BD40" s="34"/>
       <c r="BR40" s="22" t="s">
         <v>39</v>
       </c>
       <c r="BS40" s="17">
         <f>+Main!G4</f>
-        <v>2598</v>
-      </c>
-    </row>
-    <row r="41" spans="2:73">
+        <v>2904.98</v>
+      </c>
+    </row>
+    <row r="41" spans="2:71">
       <c r="B41" s="30"/>
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
@@ -8348,7 +8383,7 @@
       <c r="BR41" s="45"/>
       <c r="BS41" s="45"/>
     </row>
-    <row r="42" spans="2:73" s="31" customFormat="1">
+    <row r="42" spans="2:71" s="31" customFormat="1">
       <c r="B42" s="10"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
@@ -8383,7 +8418,7 @@
       <c r="BR42" s="22"/>
       <c r="BS42" s="17"/>
     </row>
-    <row r="43" spans="2:73" s="31" customFormat="1">
+    <row r="43" spans="2:71" s="31" customFormat="1">
       <c r="B43" s="10"/>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
@@ -8420,10 +8455,10 @@
       </c>
       <c r="BS43" s="23">
         <f>+BS39/BS40-1</f>
-        <v>-1.6343278615309154E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:73" s="44" customFormat="1">
+        <v>-0.12028992896425206</v>
+      </c>
+    </row>
+    <row r="44" spans="2:71" s="44" customFormat="1">
       <c r="B44" s="10" t="s">
         <v>167</v>
       </c>
@@ -8452,7 +8487,7 @@
       </c>
       <c r="X44" s="45">
         <f>+BS40</f>
-        <v>2598</v>
+        <v>2904.98</v>
       </c>
       <c r="Y44" s="45"/>
       <c r="Z44" s="45"/>
@@ -8499,7 +8534,7 @@
       <c r="BR44" s="20"/>
       <c r="BS44" s="20"/>
     </row>
-    <row r="45" spans="2:73" s="44" customFormat="1">
+    <row r="45" spans="2:71" s="44" customFormat="1">
       <c r="B45" s="10" t="s">
         <v>168</v>
       </c>
@@ -8533,7 +8568,7 @@
       </c>
       <c r="X45" s="45">
         <f>+Main!G6/1000</f>
-        <v>71240197.062000006</v>
+        <v>79657947.52161999</v>
       </c>
       <c r="Y45" s="45"/>
       <c r="Z45" s="45"/>
@@ -8580,7 +8615,7 @@
       <c r="BR45" s="20"/>
       <c r="BS45" s="20"/>
     </row>
-    <row r="46" spans="2:73" s="44" customFormat="1">
+    <row r="46" spans="2:71" s="44" customFormat="1">
       <c r="B46" s="10" t="s">
         <v>169</v>
       </c>
@@ -8614,7 +8649,7 @@
       </c>
       <c r="X46" s="45">
         <f>+Main!G9/1000</f>
-        <v>70679588.062000006</v>
+        <v>79097338.52161999</v>
       </c>
       <c r="Y46" s="45"/>
       <c r="Z46" s="45"/>
@@ -8659,7 +8694,7 @@
       <c r="BM46" s="24"/>
       <c r="BN46" s="24"/>
     </row>
-    <row r="47" spans="2:73" s="31" customFormat="1">
+    <row r="47" spans="2:71" s="31" customFormat="1">
       <c r="B47" s="10"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -8692,7 +8727,7 @@
       <c r="BM47" s="55"/>
       <c r="BN47" s="55"/>
     </row>
-    <row r="48" spans="2:73" s="31" customFormat="1">
+    <row r="48" spans="2:71" s="31" customFormat="1">
       <c r="B48" s="10"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>

</xml_diff>